<commit_message>
evo: TBS merged fields
</commit_message>
<xml_diff>
--- a/templates/trunk/templates/styles/office/demo_spreadsheet_msoffice.xlsx
+++ b/templates/trunk/templates/styles/office/demo_spreadsheet_msoffice.xlsx
@@ -16,9 +16,192 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>MAARCH</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>Contact externe: Civilité</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_TITLE]</t>
+  </si>
+  <si>
+    <t>Contact externe: Nom</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_LASTNAME]</t>
+  </si>
+  <si>
+    <t>Contact externe: Prénom</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_FIRSTNAME]</t>
+  </si>
+  <si>
+    <t>Contact externe : Organisation</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_SOCIETY]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse N°</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_NUM]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Rue</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_STREET]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Complement</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_COMP]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Ville</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_TOWN]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse CP</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_PC]</t>
+  </si>
+  <si>
+    <t>Contact externe : Adresse Pays</t>
+  </si>
+  <si>
+    <t>[onshow.CONTACT_ADRS_COUNTRY]</t>
+  </si>
+  <si>
+    <t>Contact interne: Nom</t>
+  </si>
+  <si>
+    <t>[onshow.USER_LASTNAME]</t>
+  </si>
+  <si>
+    <t>Contact interne: Prénom</t>
+  </si>
+  <si>
+    <t>[onshow.USER_FIRSTNAME]</t>
+  </si>
+  <si>
+    <t>Courrier: Service Traitant</t>
+  </si>
+  <si>
+    <t>[onshow.DESTINATION]</t>
+  </si>
+  <si>
+    <t>Courrier: Type de document</t>
+  </si>
+  <si>
+    <t>[onshow.DOCTYPE]</t>
+  </si>
+  <si>
+    <t>Courrier: Catégorie</t>
+  </si>
+  <si>
+    <t>[onshow.CAT_ID]</t>
+  </si>
+  <si>
+    <t>Courrier: Nature</t>
+  </si>
+  <si>
+    <t>[onshow.NATURE]</t>
+  </si>
+  <si>
+    <t>Courrier: Date d'arrivée</t>
+  </si>
+  <si>
+    <t>[onshow.ADMISSION_DATE]</t>
+  </si>
+  <si>
+    <t>Courrier: Date du courrier</t>
+  </si>
+  <si>
+    <t>[onshow.DOC_DATE]</t>
+  </si>
+  <si>
+    <t>Courrier: Date limite de traitement</t>
+  </si>
+  <si>
+    <t>[onshow.PROCESS_LIMIT_DATE]</t>
+  </si>
+  <si>
+    <t>Courrier: Notes de traitement</t>
+  </si>
+  <si>
+    <t>[onshow.PROCESS_NOTES]</t>
+  </si>
+  <si>
+    <t>Courrier: Date de clôture</t>
+  </si>
+  <si>
+    <t>[onshow.CLOSING_DATE]</t>
+  </si>
+  <si>
+    <t>Courrier: Objet</t>
+  </si>
+  <si>
+    <t>[onshow.SUBJECT]</t>
+  </si>
+  <si>
+    <t>Courrier: Numéro chrono</t>
+  </si>
+  <si>
+    <t>[onshow.CHRONO]</t>
+  </si>
+  <si>
+    <t>Document: Auteur</t>
+  </si>
+  <si>
+    <t>[onshow.AUTHOR]</t>
+  </si>
+  <si>
+    <t>Document: Date d'enregistrement</t>
+  </si>
+  <si>
+    <t>[onshow.CREATION_DATE]</t>
+  </si>
+  <si>
+    <t>Special: Date du jour</t>
+  </si>
+  <si>
+    <t>[onshow.NOW]</t>
+  </si>
+  <si>
+    <t>Special: Nom du destinataire traitant</t>
+  </si>
+  <si>
+    <t>[onshow.CURRENT_USER_LASTNAME]</t>
+  </si>
+  <si>
+    <t>Special: Prénom du destinataire traitant</t>
+  </si>
+  <si>
+    <t>[onshow.CURRENT_USER_FIRSTNAME]</t>
+  </si>
+  <si>
+    <t>Special: Téléphone du destinataire traitant</t>
+  </si>
+  <si>
+    <t>[onshow.CURRENT_USER_PHONE]</t>
+  </si>
+  <si>
+    <t>Special: Mail du destinataire traitant</t>
+  </si>
+  <si>
+    <t>[onshow.CURRENT_USER_EMAIL]</t>
   </si>
 </sst>
 </file>
@@ -357,17 +540,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
evo: new merge fields
</commit_message>
<xml_diff>
--- a/templates/trunk/templates/styles/office/demo_spreadsheet_msoffice.xlsx
+++ b/templates/trunk/templates/styles/office/demo_spreadsheet_msoffice.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>NAME</t>
   </si>
@@ -27,181 +27,175 @@
     <t>Contact externe: Civilité</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_TITLE]</t>
-  </si>
-  <si>
     <t>Contact externe: Nom</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_LASTNAME]</t>
-  </si>
-  <si>
     <t>Contact externe: Prénom</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_FIRSTNAME]</t>
-  </si>
-  <si>
     <t>Contact externe : Organisation</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_SOCIETY]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse N°</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_NUM]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Rue</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_STREET]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Complement</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_COMP]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Ville</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_TOWN]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse CP</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_PC]</t>
-  </si>
-  <si>
     <t>Contact externe : Adresse Pays</t>
   </si>
   <si>
-    <t>[onshow.CONTACT_ADRS_COUNTRY]</t>
-  </si>
-  <si>
     <t>Contact interne: Nom</t>
   </si>
   <si>
-    <t>[onshow.USER_LASTNAME]</t>
-  </si>
-  <si>
     <t>Contact interne: Prénom</t>
   </si>
   <si>
-    <t>[onshow.USER_FIRSTNAME]</t>
-  </si>
-  <si>
     <t>Courrier: Service Traitant</t>
   </si>
   <si>
-    <t>[onshow.DESTINATION]</t>
-  </si>
-  <si>
     <t>Courrier: Type de document</t>
   </si>
   <si>
-    <t>[onshow.DOCTYPE]</t>
-  </si>
-  <si>
     <t>Courrier: Catégorie</t>
   </si>
   <si>
-    <t>[onshow.CAT_ID]</t>
-  </si>
-  <si>
     <t>Courrier: Nature</t>
   </si>
   <si>
-    <t>[onshow.NATURE]</t>
-  </si>
-  <si>
     <t>Courrier: Date d'arrivée</t>
   </si>
   <si>
-    <t>[onshow.ADMISSION_DATE]</t>
-  </si>
-  <si>
     <t>Courrier: Date du courrier</t>
   </si>
   <si>
-    <t>[onshow.DOC_DATE]</t>
-  </si>
-  <si>
     <t>Courrier: Date limite de traitement</t>
   </si>
   <si>
-    <t>[onshow.PROCESS_LIMIT_DATE]</t>
-  </si>
-  <si>
     <t>Courrier: Notes de traitement</t>
   </si>
   <si>
-    <t>[onshow.PROCESS_NOTES]</t>
-  </si>
-  <si>
     <t>Courrier: Date de clôture</t>
   </si>
   <si>
-    <t>[onshow.CLOSING_DATE]</t>
-  </si>
-  <si>
     <t>Courrier: Objet</t>
   </si>
   <si>
-    <t>[onshow.SUBJECT]</t>
-  </si>
-  <si>
     <t>Courrier: Numéro chrono</t>
   </si>
   <si>
-    <t>[onshow.CHRONO]</t>
-  </si>
-  <si>
     <t>Document: Auteur</t>
   </si>
   <si>
-    <t>[onshow.AUTHOR]</t>
-  </si>
-  <si>
     <t>Document: Date d'enregistrement</t>
   </si>
   <si>
-    <t>[onshow.CREATION_DATE]</t>
-  </si>
-  <si>
     <t>Special: Date du jour</t>
   </si>
   <si>
-    <t>[onshow.NOW]</t>
-  </si>
-  <si>
     <t>Special: Nom du destinataire traitant</t>
   </si>
   <si>
-    <t>[onshow.CURRENT_USER_LASTNAME]</t>
-  </si>
-  <si>
     <t>Special: Prénom du destinataire traitant</t>
   </si>
   <si>
-    <t>[onshow.CURRENT_USER_FIRSTNAME]</t>
-  </si>
-  <si>
     <t>Special: Téléphone du destinataire traitant</t>
   </si>
   <si>
-    <t>[onshow.CURRENT_USER_PHONE]</t>
-  </si>
-  <si>
     <t>Special: Mail du destinataire traitant</t>
   </si>
   <si>
-    <t>[onshow.CURRENT_USER_EMAIL]</t>
+    <t>[contact.title]</t>
+  </si>
+  <si>
+    <t>[contact.lastname]</t>
+  </si>
+  <si>
+    <t>[contact.firstname]</t>
+  </si>
+  <si>
+    <t>[contact.society]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_num]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_street]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_comp]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_town]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_pc]</t>
+  </si>
+  <si>
+    <t>[contact.adrs_contry]</t>
+  </si>
+  <si>
+    <t>[user.lastname]</t>
+  </si>
+  <si>
+    <t>[user.firstname]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.destination]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.doctype]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.category_id]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.nature]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.admission_date]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.doc_date]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.process_limit_date]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.process_notes]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.closing_date]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.subject]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.chrono]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.author]</t>
+  </si>
+  <si>
+    <t>[res_letterbox.creation_date]</t>
+  </si>
+  <si>
+    <t>[system.now]</t>
+  </si>
+  <si>
+    <t>[user.phone]</t>
+  </si>
+  <si>
+    <t>[user.mail]</t>
   </si>
 </sst>
 </file>
@@ -543,7 +537,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,239 +559,239 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>